<commit_message>
Documentatie: Testverslag 2.xlsx bijgewerkt (blad: Management Interface).
</commit_message>
<xml_diff>
--- a/Documentatie/Testplan/Testverslag 2.xlsx
+++ b/Documentatie/Testplan/Testverslag 2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="18195" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="18195" windowHeight="7995" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Controller (Server)" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="66">
   <si>
     <t>Punten</t>
   </si>
@@ -165,18 +165,6 @@
     <t>Website past zich aan aan het scherm!</t>
   </si>
   <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>Firefox</t>
-  </si>
-  <si>
-    <t>Safari</t>
-  </si>
-  <si>
-    <t>Internet Explorer</t>
-  </si>
-  <si>
     <t>Data ophalen vanuit de statistics.json file in de uploads map</t>
   </si>
   <si>
@@ -208,13 +196,37 @@
   </si>
   <si>
     <t>Ze spawnen momenteel nog buiten de map</t>
+  </si>
+  <si>
+    <t>PC / Chrome</t>
+  </si>
+  <si>
+    <t>PC / Safari</t>
+  </si>
+  <si>
+    <t>PC / Firefox</t>
+  </si>
+  <si>
+    <t>PC / Internet Explorer</t>
+  </si>
+  <si>
+    <t>Android / AndroidBrowser (Internet)</t>
+  </si>
+  <si>
+    <t>Android / Chrome</t>
+  </si>
+  <si>
+    <t>iOS / Safari</t>
+  </si>
+  <si>
+    <t>iOS / Chrome</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,7 +394,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -456,6 +468,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -490,6 +503,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -665,14 +679,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
@@ -681,17 +695,17 @@
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F2" s="9"/>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>20</v>
       </c>
@@ -700,14 +714,14 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -724,7 +738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="45">
+    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -739,7 +753,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
@@ -756,7 +770,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="75">
+    <row r="10" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
@@ -773,9 +787,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="90">
+    <row r="11" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>10</v>
@@ -790,7 +804,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="90">
+    <row r="12" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
@@ -807,9 +821,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="90">
+    <row r="13" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>15</v>
@@ -822,84 +836,84 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="3"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="3"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="3"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="3"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="3"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -918,14 +932,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
@@ -934,17 +948,17 @@
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F2" s="9"/>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>23</v>
       </c>
@@ -953,14 +967,14 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -977,7 +991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="45">
+    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -992,123 +1006,123 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="45">
+    <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="3"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="2:6" ht="60">
+    <row r="10" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="3"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="3"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="3"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="3"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="3"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="3"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="3"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="3"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1127,14 +1141,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
@@ -1143,17 +1157,17 @@
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F2" s="9"/>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
@@ -1162,14 +1176,14 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1186,7 +1200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="45">
+    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1201,7 +1215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>26</v>
       </c>
@@ -1210,7 +1224,7 @@
       <c r="E9" s="11"/>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="2:6" ht="45">
+    <row r="10" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1225,7 +1239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="45">
+    <row r="11" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
@@ -1240,7 +1254,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>31</v>
       </c>
@@ -1249,7 +1263,7 @@
       <c r="E12" s="11"/>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="2:6" ht="30">
+    <row r="13" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
@@ -1264,7 +1278,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="60">
+    <row r="14" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
@@ -1279,7 +1293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="60">
+    <row r="15" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>36</v>
       </c>
@@ -1294,7 +1308,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
         <v>38</v>
       </c>
@@ -1303,7 +1317,7 @@
       <c r="E16" s="11"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>39</v>
       </c>
@@ -1311,7 +1325,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E17" s="3">
         <v>41617</v>
@@ -1320,7 +1334,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="45">
+    <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>40</v>
       </c>
@@ -1328,7 +1342,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E18" s="3">
         <v>41625</v>
@@ -1337,7 +1351,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="30">
+    <row r="19" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
@@ -1350,7 +1364,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="30">
+    <row r="20" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>42</v>
       </c>
@@ -1363,7 +1377,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="30">
+    <row r="21" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>43</v>
       </c>
@@ -1376,7 +1390,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="30">
+    <row r="22" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>44</v>
       </c>
@@ -1389,21 +1403,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="3"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1425,14 +1439,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
@@ -1441,17 +1455,17 @@
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F2" s="9"/>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
@@ -1460,13 +1474,13 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1483,7 +1497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="45">
+    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1498,7 +1512,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="45">
+    <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
@@ -1515,7 +1529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>45</v>
       </c>
@@ -1532,9 +1546,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="75">
+    <row r="11" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>10</v>
@@ -1547,9 +1561,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="45">
+    <row r="12" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>10</v>
@@ -1562,18 +1576,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>10</v>
@@ -1586,9 +1600,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>10</v>
@@ -1601,9 +1615,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>10</v>
@@ -1616,9 +1630,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="30">
+    <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>10</v>
@@ -1631,56 +1645,88 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+    <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="E18" s="3">
+        <v>41624</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="2:6">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="E19" s="3">
+        <v>41624</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="E20" s="3">
+        <v>41624</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="2:6">
+      <c r="E21" s="3">
+        <v>41624</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="3"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="3"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>

</xml_diff>

<commit_message>
Documentatie: Update Testverslag 2.xlsx
</commit_message>
<xml_diff>
--- a/Documentatie/Testplan/Testverslag 2.xlsx
+++ b/Documentatie/Testplan/Testverslag 2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="18195" windowHeight="7995" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="18195" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Controller (Server)" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="67">
   <si>
     <t>Punten</t>
   </si>
@@ -195,9 +195,6 @@
     <t>Ze kunnen al aangemaakt worden</t>
   </si>
   <si>
-    <t>Ze spawnen momenteel nog buiten de map</t>
-  </si>
-  <si>
     <t>PC / Chrome</t>
   </si>
   <si>
@@ -220,13 +217,19 @@
   </si>
   <si>
     <t>iOS / Chrome</t>
+  </si>
+  <si>
+    <t>Ze rijden al wel alleen nog niet naar de juiste locatie!</t>
+  </si>
+  <si>
+    <t>Nog niet aangewerkt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,7 +397,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -468,7 +471,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -503,7 +505,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -679,14 +680,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
@@ -695,7 +696,7 @@
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6">
       <c r="B2" s="7" t="s">
         <v>53</v>
       </c>
@@ -705,7 +706,7 @@
       </c>
       <c r="F2" s="9"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6">
       <c r="B5" s="6" t="s">
         <v>20</v>
       </c>
@@ -714,14 +715,14 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -738,7 +739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="45">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -753,7 +754,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6">
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
@@ -770,7 +771,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="75">
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
@@ -787,7 +788,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="90">
       <c r="B11" s="2" t="s">
         <v>50</v>
       </c>
@@ -804,7 +805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="90">
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
@@ -821,7 +822,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="90">
       <c r="B13" s="2" t="s">
         <v>55</v>
       </c>
@@ -836,84 +837,84 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="3"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="3"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="3"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="3"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="3"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -932,14 +933,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
@@ -948,7 +949,7 @@
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6">
       <c r="B2" s="7" t="s">
         <v>53</v>
       </c>
@@ -958,7 +959,7 @@
       </c>
       <c r="F2" s="9"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6">
       <c r="B5" s="6" t="s">
         <v>23</v>
       </c>
@@ -967,14 +968,14 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -991,7 +992,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="45">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1006,7 +1007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="45">
       <c r="B9" s="2" t="s">
         <v>51</v>
       </c>
@@ -1015,7 +1016,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="60">
       <c r="B10" s="2" t="s">
         <v>52</v>
       </c>
@@ -1024,105 +1025,105 @@
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="3"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="3"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="3"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="3"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="3"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="3"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="3"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="3"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1141,14 +1142,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
@@ -1157,7 +1158,7 @@
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6">
       <c r="B2" s="7" t="s">
         <v>53</v>
       </c>
@@ -1167,7 +1168,7 @@
       </c>
       <c r="F2" s="9"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6">
       <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
@@ -1176,14 +1177,14 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1200,7 +1201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="45">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1215,7 +1216,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6">
       <c r="B9" s="10" t="s">
         <v>26</v>
       </c>
@@ -1224,7 +1225,7 @@
       <c r="E9" s="11"/>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="45">
       <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1239,7 +1240,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="45">
       <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
@@ -1254,7 +1255,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6">
       <c r="B12" s="10" t="s">
         <v>31</v>
       </c>
@@ -1263,7 +1264,7 @@
       <c r="E12" s="11"/>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="30">
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
@@ -1278,7 +1279,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="60">
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
@@ -1293,7 +1294,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="60">
       <c r="B15" s="2" t="s">
         <v>36</v>
       </c>
@@ -1308,7 +1309,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6">
       <c r="B16" s="10" t="s">
         <v>38</v>
       </c>
@@ -1317,7 +1318,7 @@
       <c r="E16" s="11"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6">
       <c r="B17" s="2" t="s">
         <v>39</v>
       </c>
@@ -1334,16 +1335,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="45">
       <c r="B18" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>57</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="3">
         <v>41625</v>
       </c>
@@ -1351,33 +1350,39 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="30">
       <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="3"/>
+      <c r="D19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="3">
+        <v>41631</v>
+      </c>
       <c r="F19" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" ht="30">
       <c r="B20" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" ht="30">
       <c r="B21" s="2" t="s">
         <v>43</v>
       </c>
@@ -1390,7 +1395,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" ht="30">
       <c r="B22" s="2" t="s">
         <v>44</v>
       </c>
@@ -1403,21 +1408,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="3"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1439,14 +1444,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
@@ -1455,7 +1460,7 @@
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6">
       <c r="B2" s="7" t="s">
         <v>53</v>
       </c>
@@ -1465,7 +1470,7 @@
       </c>
       <c r="F2" s="9"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6">
       <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
@@ -1474,13 +1479,13 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6">
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1497,7 +1502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="45">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1512,7 +1517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="45">
       <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
@@ -1529,7 +1534,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6">
       <c r="B10" s="2" t="s">
         <v>45</v>
       </c>
@@ -1546,7 +1551,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="75">
       <c r="B11" s="2" t="s">
         <v>47</v>
       </c>
@@ -1561,7 +1566,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="45">
       <c r="B12" s="2" t="s">
         <v>48</v>
       </c>
@@ -1576,7 +1581,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6">
       <c r="B13" s="10" t="s">
         <v>49</v>
       </c>
@@ -1585,9 +1590,9 @@
       <c r="E13" s="11"/>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6">
       <c r="B14" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>10</v>
@@ -1600,9 +1605,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6">
       <c r="B15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>10</v>
@@ -1615,9 +1620,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6">
       <c r="B16" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>10</v>
@@ -1630,9 +1635,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="30">
       <c r="B17" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>10</v>
@@ -1645,9 +1650,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="45">
       <c r="B18" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>10</v>
@@ -1660,9 +1665,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="30">
       <c r="B19" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>10</v>
@@ -1675,9 +1680,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6">
       <c r="B20" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>10</v>
@@ -1690,9 +1695,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6">
       <c r="B21" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>10</v>
@@ -1705,28 +1710,28 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="3"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="3"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>

</xml_diff>

<commit_message>
Documentatie: Testverslag 2.xlsx bijgewerkt (deze versie is gestuurd naar Jos en Fiona).
</commit_message>
<xml_diff>
--- a/Documentatie/Testplan/Testverslag 2.xlsx
+++ b/Documentatie/Testplan/Testverslag 2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="18195" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="18195" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Controller (Server)" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="67">
   <si>
     <t>Punten</t>
   </si>
@@ -216,20 +216,20 @@
     <t>iOS / Chrome</t>
   </si>
   <si>
-    <t>Ze rijden al wel alleen nog niet naar de juiste locatie!</t>
-  </si>
-  <si>
-    <t>Nog niet aangewerkt</t>
-  </si>
-  <si>
-    <t>Met een vector, die vanuit het protocol wordt gestuurd, werkt dit.</t>
+    <t>Nog niet aangewerkt.</t>
+  </si>
+  <si>
+    <t>Ze rijden al wel alleen nog niet naar de juiste locatie.</t>
+  </si>
+  <si>
+    <t>Met een vector, die vanuit het protocol wordt gestuurd, werkt dit!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,7 +397,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -471,6 +471,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -505,6 +506,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -680,14 +682,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
@@ -696,7 +698,7 @@
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>52</v>
       </c>
@@ -706,7 +708,7 @@
       </c>
       <c r="F2" s="9"/>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>20</v>
       </c>
@@ -715,14 +717,14 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -739,7 +741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="45">
+    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -754,7 +756,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
@@ -771,7 +773,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="75">
+    <row r="10" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
@@ -788,7 +790,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="90">
+    <row r="11" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>49</v>
       </c>
@@ -805,7 +807,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="90">
+    <row r="12" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
@@ -822,7 +824,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="90">
+    <row r="13" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>54</v>
       </c>
@@ -837,84 +839,84 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="3"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="3"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="3"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="3"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="3"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -933,14 +935,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
@@ -949,7 +951,7 @@
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>52</v>
       </c>
@@ -959,7 +961,7 @@
       </c>
       <c r="F2" s="9"/>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>23</v>
       </c>
@@ -968,14 +970,14 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -992,7 +994,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="45">
+    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1007,123 +1009,131 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="45">
+    <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3">
+        <v>41624</v>
+      </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="2:6" ht="60">
+    <row r="10" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3">
+        <v>41624</v>
+      </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="3"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="3"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="3"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="3"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="3"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="3"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="3"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="3"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1142,14 +1152,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
@@ -1158,7 +1168,7 @@
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>52</v>
       </c>
@@ -1168,7 +1178,7 @@
       </c>
       <c r="F2" s="9"/>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
@@ -1177,14 +1187,14 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1201,7 +1211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="45">
+    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1216,7 +1226,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>26</v>
       </c>
@@ -1225,7 +1235,7 @@
       <c r="E9" s="11"/>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="2:6" ht="45">
+    <row r="10" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1242,7 +1252,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="45">
+    <row r="11" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
@@ -1257,7 +1267,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>31</v>
       </c>
@@ -1266,7 +1276,7 @@
       <c r="E12" s="11"/>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="2:6" ht="30">
+    <row r="13" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
@@ -1281,7 +1291,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="60">
+    <row r="14" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>34</v>
       </c>
@@ -1296,7 +1306,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="60">
+    <row r="15" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
@@ -1311,7 +1321,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
         <v>37</v>
       </c>
@@ -1320,7 +1330,7 @@
       <c r="E16" s="11"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>38</v>
       </c>
@@ -1337,7 +1347,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="45">
+    <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>39</v>
       </c>
@@ -1352,7 +1362,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="30">
+    <row r="19" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>40</v>
       </c>
@@ -1360,7 +1370,7 @@
         <v>15</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E19" s="3">
         <v>41631</v>
@@ -1369,7 +1379,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="30">
+    <row r="20" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>41</v>
       </c>
@@ -1377,14 +1387,14 @@
         <v>15</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="30">
+    <row r="21" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>42</v>
       </c>
@@ -1397,7 +1407,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="30">
+    <row r="22" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>43</v>
       </c>
@@ -1410,21 +1420,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="3"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1446,14 +1456,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
@@ -1462,7 +1472,7 @@
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>52</v>
       </c>
@@ -1472,7 +1482,7 @@
       </c>
       <c r="F2" s="9"/>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
@@ -1481,13 +1491,13 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1504,7 +1514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="45">
+    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1519,7 +1529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="45">
+    <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
@@ -1536,7 +1546,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>44</v>
       </c>
@@ -1553,7 +1563,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="75">
+    <row r="11" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>46</v>
       </c>
@@ -1568,7 +1578,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="45">
+    <row r="12" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>47</v>
       </c>
@@ -1583,7 +1593,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>48</v>
       </c>
@@ -1592,7 +1602,7 @@
       <c r="E13" s="11"/>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>56</v>
       </c>
@@ -1607,7 +1617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>57</v>
       </c>
@@ -1622,7 +1632,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>58</v>
       </c>
@@ -1637,7 +1647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="30">
+    <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>59</v>
       </c>
@@ -1652,7 +1662,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="45">
+    <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>60</v>
       </c>
@@ -1667,7 +1677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="30">
+    <row r="19" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>61</v>
       </c>
@@ -1682,7 +1692,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>62</v>
       </c>
@@ -1697,7 +1707,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>63</v>
       </c>
@@ -1712,28 +1722,28 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="3"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="3"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>

</xml_diff>